<commit_message>
Updated Migration Wave to filtered returning results as data taken from the output of the previous agent
</commit_message>
<xml_diff>
--- a/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
+++ b/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
@@ -718,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB278"/>
+  <dimension ref="A1:AB279"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -2523,6 +2523,123 @@
       <c r="P278" s="12" t="n"/>
       <c r="V278" s="12" t="n"/>
     </row>
+    <row r="279">
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Karapakkam</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="O279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="V279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="W279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="X279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Y279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Z279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AA279" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB17"/>
   <conditionalFormatting sqref="P17">

</xml_diff>

<commit_message>
Updated Excel file with new migration wave data from Agent-2 output
</commit_message>
<xml_diff>
--- a/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
+++ b/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
@@ -718,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB279"/>
+  <dimension ref="A1:BD280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -760,7 +760,7 @@
     <row r="1" ht="48.75" customFormat="1" customHeight="1" s="7">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hotcarding Spreadsheet - Migration Wave </t>
+          <t>Hotcarding Spreadsheet - Migration Wave 11/26/2025</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1043,12 +1043,152 @@
       </c>
       <c r="AA2" s="8" t="inlineStr">
         <is>
-          <t>Migration Team?</t>
+          <t>Hotcarding Spreadsheet Migration Wave</t>
         </is>
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>Migration Team?</t>
+          <t>Issuer Address</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Zipcode</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Fi Name</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>Fi Contact</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>Visa Bid</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Mc Ica</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>New Mc Ica New Berlin</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>Bin</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>Bin Type Consumer Business Atm</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>Pan Length 16 17 18 19</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>Real R T</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>Pseudo R T</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>Aims Id</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>Issuing Network Participation Plus Cirrus Pulse Remember Jeanie Nyce Nycejp53 Nyce Sum Column Aa Y Jadv Nyce Sum Column Aa Y</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>Acquiring Network Participation Nyce Interlink Star Remember Jeanie Nyce Nycejp53 Nyce Sum Column Aa Y Jadv Nyce Sum Column Aa Y</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>Vau Segment Id</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>Existing Plus Rid To Be Deleted</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>Mc Affiliate Id</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>Ach Account For Billing And Fees Dda Only</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>Ach R T For Billing And Fees</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>Dda Versus Gl</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>Regional Networks Interchange Account</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>Regional Networks Interchange R T</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>Dda Versus Gl 1</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t>New Platform</t>
         </is>
       </c>
     </row>
@@ -2732,6 +2872,163 @@
         </is>
       </c>
     </row>
+    <row r="280">
+      <c r="X280" t="inlineStr">
+        <is>
+          <t>11/26/2025</t>
+        </is>
+      </c>
+      <c r="AA280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AB280" t="inlineStr">
+        <is>
+          <t>Karapakkam</t>
+        </is>
+      </c>
+      <c r="AC280" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="AD280" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="AE280" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
+      <c r="AF280" t="inlineStr">
+        <is>
+          <t>xxxxyyyyyy</t>
+        </is>
+      </c>
+      <c r="AG280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AH280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AI280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AJ280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AK280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AL280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AM280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AN280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AO280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AP280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AQ280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AR280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AS280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AT280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AU280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AV280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AW280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AZ280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BA280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BB280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BC280" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="BD280" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB17"/>
   <conditionalFormatting sqref="P17">

</xml_diff>

<commit_message>
Updated Excel file with new data from Agent-2 output
</commit_message>
<xml_diff>
--- a/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
+++ b/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
@@ -718,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC279"/>
+  <dimension ref="A1:BF280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -1178,12 +1178,27 @@
       </c>
       <c r="BB2" t="inlineStr">
         <is>
-          <t>Switch</t>
+          <t>Wave001</t>
         </is>
       </c>
       <c r="BC2" t="inlineStr">
         <is>
-          <t>New Platform</t>
+          <t>Wave002</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t>Wave003</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>Wave004</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>Wave005</t>
         </is>
       </c>
     </row>
@@ -2739,9 +2754,6 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="AP279" t="inlineStr"/>
-      <c r="AQ279" t="inlineStr"/>
-      <c r="AR279" t="inlineStr"/>
       <c r="AS279" t="inlineStr">
         <is>
           <t>NA</t>
@@ -2795,6 +2807,43 @@
       <c r="BC279" t="inlineStr">
         <is>
           <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="AZ280" t="inlineStr">
+        <is>
+          <t>FISB</t>
+        </is>
+      </c>
+      <c r="BA280" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="BB280" t="inlineStr">
+        <is>
+          <t>ValueA</t>
+        </is>
+      </c>
+      <c r="BC280" t="inlineStr">
+        <is>
+          <t>ValueB</t>
+        </is>
+      </c>
+      <c r="BD280" t="inlineStr">
+        <is>
+          <t>ValueC</t>
+        </is>
+      </c>
+      <c r="BE280" t="inlineStr">
+        <is>
+          <t>ValueD</t>
+        </is>
+      </c>
+      <c r="BF280" t="inlineStr">
+        <is>
+          <t>ValueE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Append migration wave row for 11/26/2025 to Wave_____ sheet
</commit_message>
<xml_diff>
--- a/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
+++ b/python/Wave-Network & Licensing Request Form Norcross Migrations.xlsx
@@ -718,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB278"/>
+  <dimension ref="A1:AK278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -917,6 +917,51 @@
           <t>DDA versus GL</t>
         </is>
       </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>ADDRESS</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>ZIP CODE</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>ENTITY NAME (DN)</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>FI PRIMARY CONTACT NAME</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>FI PRIMARY CONTACT EMAIL</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>BINs</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>BIN LENGTH</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>ISSUING NETWORKS</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>ACQUIRING NETWORKS</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="17.25" customFormat="1" customHeight="1" s="11">
       <c r="A2" s="8" t="inlineStr">
@@ -1151,16 +1196,142 @@
       <c r="AB3" s="17" t="n"/>
     </row>
     <row r="4" customFormat="1" s="18">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>11/26/2025</t>
+        </is>
+      </c>
       <c r="B4" s="19" t="n"/>
-      <c r="C4" s="19" t="n"/>
+      <c r="C4" s="19" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
       <c r="F4" s="20" t="n"/>
       <c r="G4" s="20" t="n"/>
       <c r="H4" s="21" t="n"/>
-      <c r="P4" s="22" t="n"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>PaymentsOne Debit</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P4" s="22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="S4" s="12" t="n"/>
-      <c r="Z4" s="23" t="n"/>
-      <c r="AA4" s="23" t="n"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Z4" s="23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AA4" s="23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
       <c r="AB4" s="23" t="n"/>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Karapakkam</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>xxxxyyyyyy</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="5" customFormat="1" s="18">
       <c r="A5" s="12" t="n"/>

</xml_diff>